<commit_message>
Data number of poles
</commit_message>
<xml_diff>
--- a/Results/increasingGamma/NonClassical/nuOfPoles_increasingGamma_NonClassic.xlsx
+++ b/Results/increasingGamma/NonClassical/nuOfPoles_increasingGamma_NonClassic.xlsx
@@ -111,10 +111,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:S32"/>
+  <dimension ref="A2:T32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="293" zoomScaleNormal="293" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="293" zoomScaleNormal="293" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U32" activeCellId="0" sqref="U2:U32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -180,6 +180,9 @@
       <c r="S2" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="T2" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -239,6 +242,9 @@
       <c r="S3" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="T3" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -298,6 +304,9 @@
       <c r="S4" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="T4" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -357,6 +366,9 @@
       <c r="S5" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="T5" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -416,6 +428,9 @@
       <c r="S6" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="T6" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -475,6 +490,9 @@
       <c r="S7" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="T7" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -534,6 +552,9 @@
       <c r="S8" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="T8" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -593,6 +614,9 @@
       <c r="S9" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="T9" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -652,6 +676,9 @@
       <c r="S10" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="T10" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -711,6 +738,9 @@
       <c r="S11" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="T11" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -770,6 +800,9 @@
       <c r="S12" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="T12" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -829,6 +862,9 @@
       <c r="S13" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="T13" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -888,6 +924,9 @@
       <c r="S14" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="T14" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -947,6 +986,9 @@
       <c r="S15" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="T15" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -1006,6 +1048,9 @@
       <c r="S16" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="T16" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -1065,6 +1110,9 @@
       <c r="S17" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="T17" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -1124,6 +1172,9 @@
       <c r="S18" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="T18" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -1183,6 +1234,9 @@
       <c r="S19" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="T19" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -1242,6 +1296,9 @@
       <c r="S20" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="T20" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -1301,6 +1358,9 @@
       <c r="S21" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="T21" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -1360,6 +1420,9 @@
       <c r="S22" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="T22" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -1419,6 +1482,9 @@
       <c r="S23" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="T23" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -1478,6 +1544,9 @@
       <c r="S24" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="T24" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -1537,6 +1606,9 @@
       <c r="S25" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="T25" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -1596,6 +1668,9 @@
       <c r="S26" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="T26" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -1655,6 +1730,9 @@
       <c r="S27" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="T27" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -1714,6 +1792,9 @@
       <c r="S28" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="T28" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -1773,6 +1854,9 @@
       <c r="S29" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="T29" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -1832,6 +1916,9 @@
       <c r="S30" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="T30" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -1889,6 +1976,9 @@
         <v>4</v>
       </c>
       <c r="S31" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T31" s="0" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1949,6 +2039,9 @@
       </c>
       <c r="S32" s="0" t="n">
         <v>6</v>
+      </c>
+      <c r="T32" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>